<commit_message>
update Gantt and test script
update Gantt and test script
</commit_message>
<xml_diff>
--- a/csv/JLim_UpdatedGantt-FINAL.xlsx
+++ b/csv/JLim_UpdatedGantt-FINAL.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Documents\GitHub\Capstone\csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08065E2A-25F9-4C3B-BE0B-01A64915F10A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1E2A107-F131-4F48-B38D-94973D794A41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -485,16 +485,16 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.8</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.6</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -556,16 +556,16 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1104,7 +1104,7 @@
   <dimension ref="A1:AI34"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="162" zoomScaleNormal="162" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1520,14 +1520,14 @@
       </c>
       <c r="G10" s="21">
         <f>SUM(F10*I10)</f>
-        <v>4.8</v>
+        <v>8</v>
       </c>
       <c r="H10" s="29">
         <f t="shared" ref="H10:H13" si="2">SUM(F10-G10)</f>
-        <v>3.2</v>
+        <v>0</v>
       </c>
       <c r="I10" s="22">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
@@ -1576,14 +1576,14 @@
       </c>
       <c r="G11" s="21">
         <f>SUM(F11*I11)</f>
-        <v>1.6</v>
+        <v>8</v>
       </c>
       <c r="H11" s="29">
         <f t="shared" si="2"/>
-        <v>6.4</v>
+        <v>0</v>
       </c>
       <c r="I11" s="20">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
@@ -1662,14 +1662,14 @@
       </c>
       <c r="G13" s="21">
         <f>SUM(F13*I13)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H13" s="29">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I13" s="24">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="14" spans="1:35" ht="15.75" customHeight="1">
@@ -1722,6 +1722,13 @@
     <row r="34" ht="12.75"/>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
     <mergeCell ref="I6:I7"/>
     <mergeCell ref="F6:F7"/>
     <mergeCell ref="AD6:AH6"/>
@@ -1729,13 +1736,6 @@
     <mergeCell ref="T6:X6"/>
     <mergeCell ref="J6:N6"/>
     <mergeCell ref="O6:S6"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
   </mergeCells>
   <conditionalFormatting sqref="I9:I13">
     <cfRule type="colorScale" priority="2">

</xml_diff>

<commit_message>
update char and kicking session
update char and kicking session
</commit_message>
<xml_diff>
--- a/csv/JLim_UpdatedGantt-FINAL.xlsx
+++ b/csv/JLim_UpdatedGantt-FINAL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Documents\GitHub\Capstone\csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20BC512C-FFD2-4C31-8B5F-7011F947FB3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BEF70A5-624F-45F2-86B2-B96D49EF38AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1466,7 +1466,7 @@
         <v>8</v>
       </c>
       <c r="G9" s="21">
-        <f>SUM(F9*I9)</f>
+        <f t="shared" ref="G9:G14" si="1">SUM(F9*I9)</f>
         <v>8</v>
       </c>
       <c r="H9" s="29">
@@ -1518,15 +1518,15 @@
         <v>43920</v>
       </c>
       <c r="F10" s="28">
-        <f t="shared" ref="F10:F14" si="1">DATEDIF(C10,E10,"d")+1</f>
+        <f t="shared" ref="F10:F14" si="2">DATEDIF(C10,E10,"d")+1</f>
         <v>8</v>
       </c>
       <c r="G10" s="21">
-        <f>SUM(F10*I10)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="H10" s="29">
-        <f t="shared" ref="H10:H14" si="2">SUM(F10-G10)</f>
+        <f t="shared" ref="H10:H14" si="3">SUM(F10-G10)</f>
         <v>0</v>
       </c>
       <c r="I10" s="22">
@@ -1574,15 +1574,15 @@
         <v>43927</v>
       </c>
       <c r="F11" s="28">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="G11" s="21">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="G11" s="21">
-        <f>SUM(F11*I11)</f>
-        <v>8</v>
-      </c>
       <c r="H11" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I11" s="20">
@@ -1630,15 +1630,15 @@
         <v>43934</v>
       </c>
       <c r="F12" s="28">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="G12" s="21">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="G12" s="21">
-        <f>SUM(F12*I12)</f>
-        <v>8</v>
-      </c>
       <c r="H12" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I12" s="23">
@@ -1660,15 +1660,15 @@
         <v>43941</v>
       </c>
       <c r="F13" s="28">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="G13" s="21">
         <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="G13" s="21">
-        <f>SUM(F13*I13)</f>
         <v>6.4</v>
       </c>
       <c r="H13" s="29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.5999999999999996</v>
       </c>
       <c r="I13" s="24">
@@ -1691,19 +1691,19 @@
         <v>43948</v>
       </c>
       <c r="F14" s="28">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="G14" s="21">
         <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="G14" s="21">
-        <f>SUM(F14*I14)</f>
-        <v>4</v>
+        <v>6.8</v>
       </c>
       <c r="H14" s="29">
-        <f t="shared" si="2"/>
-        <v>4</v>
+        <f t="shared" si="3"/>
+        <v>1.2000000000000002</v>
       </c>
       <c r="I14" s="24">
-        <v>0.5</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="15" spans="1:35" ht="15.75" customHeight="1">
@@ -1745,6 +1745,13 @@
     <row r="34" ht="12.75"/>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
     <mergeCell ref="I6:I7"/>
     <mergeCell ref="F6:F7"/>
     <mergeCell ref="AD6:AH6"/>
@@ -1752,13 +1759,6 @@
     <mergeCell ref="T6:X6"/>
     <mergeCell ref="J6:N6"/>
     <mergeCell ref="O6:S6"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
   </mergeCells>
   <conditionalFormatting sqref="I9:I14">
     <cfRule type="colorScale" priority="2">

</xml_diff>